<commit_message>
add municipality tax for St.Gallen
</commit_message>
<xml_diff>
--- a/data/SG/SteuerfussSG.xlsx
+++ b/data/SG/SteuerfussSG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\SG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A0BD32-07D4-4DE8-80A0-D430E6B0410C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B8B0C-4519-4A19-8874-8A10AE16C60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Kanton</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>SG</t>
+  </si>
+  <si>
+    <t>St.Gallen</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6439AF7-483B-4E31-894C-6B5766D16518}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -474,7 +477,72 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A4">
+        <v>3203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>115</v>
+      </c>
+      <c r="F4">
+        <v>141</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A5">
+        <v>3203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>115</v>
+      </c>
+      <c r="F5">
+        <v>144</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nidi/add basis tax calc for sg (#10)
* move basis calculators and rename them

* DO VARIOUS RENAMING

* add basis tax calculator for SG

* add unit test for null tax calculator

* add basis wealth tax calculator for SG

* add wealth tax calculator for SG

* support full income tax calculation for SG

* DO VARIOUS RENAMING

* FIX UNIT TESTS

* missing capital benefit calculator added

* SAVEPOINT

* FIX UNIT TESTS

* SAVEPOINT

* DO VARIOUS RENAMING

* DO VARIOUS RENAMING

* SAVEPOINT

* finalize capital benefit calc for SG

* FIX UNIT TESTS

* FIX UNIT TESTS

* fix disposed problem

* add AsNoTracking

* add mappings for DbContextOptions

* add municipality tax for St.Gallen
</commit_message>
<xml_diff>
--- a/data/SG/SteuerfussSG.xlsx
+++ b/data/SG/SteuerfussSG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\SG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A0BD32-07D4-4DE8-80A0-D430E6B0410C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B8B0C-4519-4A19-8874-8A10AE16C60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Kanton</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>SG</t>
+  </si>
+  <si>
+    <t>St.Gallen</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6439AF7-483B-4E31-894C-6B5766D16518}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -474,7 +477,72 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A4">
+        <v>3203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>2019</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>115</v>
+      </c>
+      <c r="F4">
+        <v>141</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>26</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.65">
+      <c r="A5">
+        <v>3203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>115</v>
+      </c>
+      <c r="F5">
+        <v>144</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add poll tax data
</commit_message>
<xml_diff>
--- a/data/SG/SteuerfussSG.xlsx
+++ b/data/SG/SteuerfussSG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\SG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B8B0C-4519-4A19-8874-8A10AE16C60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438F43D6-79C9-4764-966D-022A51120227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Kanton</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>St.Gallen</t>
+  </si>
+  <si>
+    <t>Personensteuer</t>
   </si>
 </sst>
 </file>
@@ -373,15 +376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6439AF7-483B-4E31-894C-6B5766D16518}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -410,10 +413,13 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A2">
         <v>3426</v>
       </c>
@@ -441,11 +447,11 @@
       <c r="I2">
         <v>24</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A3">
         <v>3426</v>
       </c>
@@ -473,11 +479,11 @@
       <c r="I3">
         <v>24</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A4">
         <v>3203</v>
       </c>
@@ -505,11 +511,11 @@
       <c r="I4">
         <v>26</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A5">
         <v>3203</v>
       </c>
@@ -537,7 +543,7 @@
       <c r="I5">
         <v>26</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nidi/add calculators for solothurn (#13)
* add income tax calculator

* change taxable amount increment from 100 to 1 for SO

* fix bug in handling tax increment which was not treated as rate in pct

* add capital benefit calculator for SO

* add personensteuer column to Steuerfuss table

* add poll tax data

* SAVEPOINT

* DO VARIOUS CLEAN-UPS

* Steuerfuss 2020 ZH

* add poll tax calculator supporting SO with tax rate on municipality level

* fix 'massgebender steuerbarer Betrag' for SO
</commit_message>
<xml_diff>
--- a/data/SG/SteuerfussSG.xlsx
+++ b/data/SG/SteuerfussSG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\SG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7B8B0C-4519-4A19-8874-8A10AE16C60F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438F43D6-79C9-4764-966D-022A51120227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Kanton</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>St.Gallen</t>
+  </si>
+  <si>
+    <t>Personensteuer</t>
   </si>
 </sst>
 </file>
@@ -373,15 +376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6439AF7-483B-4E31-894C-6B5766D16518}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -410,10 +413,13 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A2">
         <v>3426</v>
       </c>
@@ -441,11 +447,11 @@
       <c r="I2">
         <v>24</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A3">
         <v>3426</v>
       </c>
@@ -473,11 +479,11 @@
       <c r="I3">
         <v>24</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A4">
         <v>3203</v>
       </c>
@@ -505,11 +511,11 @@
       <c r="I4">
         <v>26</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.65">
       <c r="A5">
         <v>3203</v>
       </c>
@@ -537,7 +543,7 @@
       <c r="I5">
         <v>26</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>